<commit_message>
Demo Design File Updated
</commit_message>
<xml_diff>
--- a/IMS DEMO.xlsx
+++ b/IMS DEMO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meghp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazzp\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FF7916-2CF6-46F6-ADD0-3F4B3BE0D4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21779B3-AA39-4DFA-B6A8-6A3A6C8A0507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="1275" windowWidth="22935" windowHeight="12660" activeTab="3" xr2:uid="{3E622F52-6EA8-4B48-BA60-EB77EC908827}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3E622F52-6EA8-4B48-BA60-EB77EC908827}"/>
   </bookViews>
   <sheets>
     <sheet name="Side Bar" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Order" sheetId="4" r:id="rId4"/>
     <sheet name="Purches" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="170">
   <si>
     <t>Code</t>
   </si>
@@ -460,59 +460,6 @@
     <t>Initiated</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Edit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-Mail-Print-Delete</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Edit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-Mail-Print-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delete</t>
-    </r>
-  </si>
-  <si>
     <t>Drug International</t>
   </si>
   <si>
@@ -538,9 +485,6 @@
   </si>
   <si>
     <t>Purchese List</t>
-  </si>
-  <si>
-    <t>Direct Purchese</t>
   </si>
   <si>
     <t>Mail-Print-Delete</t>
@@ -639,6 +583,86 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Purches</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-P-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+  </si>
+  <si>
+    <t>E-M-P-D</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-M-P-D</t>
+    </r>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voucher </t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1102,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1153,15 +1177,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1177,9 +1249,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1195,30 +1264,6 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1228,6 +1273,42 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1246,63 +1327,37 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="60% - Accent3" xfId="7" builtinId="40"/>
@@ -1574,6 +1629,132 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5279540" y="4087345"/>
+          <a:ext cx="144421" cy="144421"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 13646"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>401079</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>39802</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>527629</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>164319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Graphic 1" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8BE5886-EDBC-4360-9630-C520D15AFCFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5277879" y="4106977"/>
+          <a:ext cx="126550" cy="124517"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>393775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28014</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>538196</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>172435</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82482204-031B-42BD-ADF8-8107C467F832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5270575" y="4095189"/>
           <a:ext cx="144421" cy="144421"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -1933,209 +2114,204 @@
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="11"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="11"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="37"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="11"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="11"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="37"/>
+      <c r="D9" s="43"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="37"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="37"/>
+      <c r="D13" s="43"/>
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="37"/>
+      <c r="D15" s="43"/>
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="37"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="37"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="37"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="37"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="37"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="37"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="37"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="37"/>
+      <c r="D29" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B8:D8"/>
@@ -2147,11 +2323,16 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId1"/>
@@ -2177,22 +2358,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2217,28 +2398,28 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48" t="s">
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48" t="s">
+      <c r="K3" s="63"/>
+      <c r="L3" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="48"/>
-      <c r="N3" s="49" t="s">
+      <c r="M3" s="63"/>
+      <c r="N3" s="64" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2255,10 +2436,10 @@
       <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="60"/>
       <c r="G4" s="6" t="s">
         <v>6</v>
       </c>
@@ -2280,7 +2461,7 @@
       <c r="M4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="49"/>
+      <c r="N4" s="64"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -2300,10 +2481,10 @@
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="44"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="4">
         <v>230</v>
       </c>
@@ -2342,10 +2523,10 @@
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="44"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="4">
         <v>3</v>
       </c>
@@ -2384,10 +2565,10 @@
       <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="44"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="4">
         <v>12</v>
       </c>
@@ -2426,10 +2607,10 @@
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="44"/>
+      <c r="F8" s="49"/>
       <c r="G8" s="4">
         <v>5</v>
       </c>
@@ -2456,57 +2637,57 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="44"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="2"/>
-      <c r="H12" s="39" t="s">
+      <c r="H12" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="39"/>
+      <c r="I12" s="55"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="42"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="F15" s="44" t="s">
+      <c r="D15" s="49"/>
+      <c r="F15" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="I15" s="44" t="s">
+      <c r="G15" s="49"/>
+      <c r="I15" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="44"/>
+      <c r="J15" s="49"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="12"/>
@@ -2519,156 +2700,156 @@
       <c r="J17" s="12"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="51"/>
+      <c r="D19" s="48"/>
       <c r="F19" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="51" t="s">
+      <c r="I19" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="51"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
       <c r="F20" s="14">
         <v>0</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44" t="s">
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="52"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="54"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="52"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55" t="s">
+      <c r="D23" s="47"/>
+      <c r="E23" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55" t="s">
+      <c r="F23" s="47"/>
+      <c r="G23" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55" t="s">
+      <c r="H23" s="47"/>
+      <c r="I23" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="55"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="56" t="s">
+      <c r="D24" s="46"/>
+      <c r="E24" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="56" t="s">
+      <c r="F24" s="46"/>
+      <c r="G24" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="57"/>
-      <c r="I24" s="56" t="s">
+      <c r="H24" s="46"/>
+      <c r="I24" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="57"/>
+      <c r="J24" s="46"/>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55" t="s">
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C26" s="56" t="s">
+      <c r="C26" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="56" t="s">
+      <c r="D26" s="46"/>
+      <c r="E26" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="56" t="s">
+      <c r="F26" s="46"/>
+      <c r="G26" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="57"/>
-      <c r="I26" s="56" t="s">
+      <c r="H26" s="46"/>
+      <c r="I26" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="J26" s="57"/>
+      <c r="J26" s="46"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55" t="s">
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="57"/>
-      <c r="E28" s="56" t="s">
+      <c r="D28" s="46"/>
+      <c r="E28" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="57"/>
-      <c r="G28" s="56" t="s">
+      <c r="F28" s="46"/>
+      <c r="G28" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="57"/>
-      <c r="I28" s="56" t="s">
+      <c r="H28" s="46"/>
+      <c r="I28" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="57"/>
+      <c r="J28" s="46"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F30" s="15" t="s">
@@ -2680,42 +2861,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="I19:J20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H13:J13"/>
@@ -2732,6 +2877,42 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:N4"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="I19:J20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2744,7 +2925,7 @@
   <dimension ref="A2:AC7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,39 +2949,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="J2" s="59" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="J2" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="S2" s="58" t="s">
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="S2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="58"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3158,34 +3339,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3DBAD4-A614-46CD-81E1-F3CCD0C29031}">
-  <dimension ref="B2:S32"/>
+  <dimension ref="B2:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20:Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
+      <c r="B2" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -3208,49 +3389,49 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="63">
+      <c r="B4" s="82">
         <v>44627</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="E4" s="63">
+      <c r="C4" s="83"/>
+      <c r="E4" s="82">
         <v>44658</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="H4" s="65" t="s">
+      <c r="F4" s="83"/>
+      <c r="H4" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="K4" s="70" t="s">
+      <c r="I4" s="85"/>
+      <c r="K4" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="71"/>
-      <c r="N4" s="70" t="s">
+      <c r="L4" s="73"/>
+      <c r="N4" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="O4" s="71"/>
-      <c r="Q4" s="70" t="s">
+      <c r="O4" s="73"/>
+      <c r="Q4" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="R4" s="71"/>
+      <c r="R4" s="73"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="O6" s="73" t="s">
+      <c r="O6" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="R6" s="62"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="81" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" s="81"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="74"/>
+      <c r="D8" s="79"/>
       <c r="E8" s="28" t="s">
         <v>114</v>
       </c>
@@ -3269,27 +3450,28 @@
       <c r="K8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="72" t="s">
+      <c r="L8" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72" t="s">
+      <c r="M8" s="37"/>
+      <c r="N8" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72" t="s">
+      <c r="O8" s="37"/>
+      <c r="P8" s="91" t="s">
         <v>119</v>
       </c>
-      <c r="R8" s="72"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="91"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="17">
         <v>123456</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="27" t="s">
         <v>121</v>
       </c>
@@ -3308,28 +3490,30 @@
       <c r="K9">
         <v>1356</v>
       </c>
-      <c r="M9" s="76" t="s">
+      <c r="L9" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="N9" s="76"/>
-      <c r="O9" s="75">
+      <c r="M9" s="39"/>
+      <c r="N9" s="38">
         <v>44599</v>
       </c>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="92" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="17">
         <v>123456</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="26" t="s">
         <v>123</v>
       </c>
@@ -3348,30 +3532,35 @@
       <c r="K10">
         <v>950</v>
       </c>
-      <c r="M10" s="76" t="s">
+      <c r="L10" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="N10" s="76"/>
-      <c r="O10" s="75">
+      <c r="M10" s="39"/>
+      <c r="N10" s="38">
         <v>44599</v>
       </c>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="95" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q10" s="95"/>
+      <c r="R10" s="93" t="s">
+        <v>163</v>
+      </c>
+      <c r="S10" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
         <v>123456</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="D11" s="44"/>
+      <c r="C11" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="49"/>
       <c r="E11" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F11">
         <v>15</v>
@@ -3388,40 +3577,42 @@
       <c r="K11">
         <v>3856</v>
       </c>
-      <c r="M11" s="76" t="s">
+      <c r="L11" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="N11" s="76"/>
-      <c r="O11" s="75">
+      <c r="M11" s="39"/>
+      <c r="N11" s="38">
         <v>44599</v>
       </c>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="95" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q11" s="95"/>
+      <c r="R11" s="94" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="67" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="67"/>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="67"/>
+      <c r="B15" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
     </row>
     <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -3429,27 +3620,27 @@
       </c>
     </row>
     <row r="17" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="78" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="K17" s="85" t="s">
-        <v>133</v>
+      <c r="B17" s="75" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="77"/>
+      <c r="K17" s="42" t="s">
+        <v>131</v>
       </c>
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
       <c r="P17" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q17" s="34"/>
     </row>
     <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="44"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="33"/>
       <c r="F19" t="s">
         <v>2</v>
@@ -3480,11 +3671,11 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="71"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="73"/>
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
       <c r="H20" s="30"/>
@@ -3496,7 +3687,7 @@
         <v>8</v>
       </c>
       <c r="M20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -3508,7 +3699,7 @@
         <v>308</v>
       </c>
       <c r="Q20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3522,10 +3713,10 @@
         <v>4</v>
       </c>
       <c r="L21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="M21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -3537,27 +3728,27 @@
         <v>308</v>
       </c>
       <c r="Q21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="81"/>
-      <c r="C22" s="82"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="68" t="s">
-        <v>152</v>
-      </c>
-      <c r="H22" s="69"/>
-      <c r="I22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
       <c r="K22" t="s">
         <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -3569,7 +3760,7 @@
         <v>308</v>
       </c>
       <c r="Q22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
@@ -3588,7 +3779,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="35" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I23" s="35" t="s">
         <v>13</v>
@@ -3597,10 +3788,10 @@
         <v>4</v>
       </c>
       <c r="L23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -3612,23 +3803,23 @@
         <v>308</v>
       </c>
       <c r="Q23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="44"/>
+      <c r="C24" s="49"/>
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="76" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="76"/>
+      <c r="E24" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="68"/>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H24" t="s">
         <v>11</v>
@@ -3640,10 +3831,10 @@
         <v>4</v>
       </c>
       <c r="L24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -3655,23 +3846,23 @@
         <v>308</v>
       </c>
       <c r="Q24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="44"/>
+      <c r="B25" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="49"/>
       <c r="D25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="76" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="76"/>
+        <v>144</v>
+      </c>
+      <c r="E25" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="68"/>
       <c r="G25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H25" t="s">
         <v>11</v>
@@ -3683,10 +3874,10 @@
         <v>4</v>
       </c>
       <c r="L25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="M25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -3698,23 +3889,23 @@
         <v>308</v>
       </c>
       <c r="Q25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="C26" s="44"/>
+      <c r="B26" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="49"/>
       <c r="D26" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="76" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="76"/>
+      <c r="E26" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="68"/>
       <c r="G26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H26" t="s">
         <v>11</v>
@@ -3726,10 +3917,10 @@
         <v>4</v>
       </c>
       <c r="L26" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -3741,21 +3932,21 @@
         <v>308</v>
       </c>
       <c r="Q26" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="44" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="44"/>
+      <c r="B27" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="49"/>
       <c r="D27" t="s">
-        <v>148</v>
-      </c>
-      <c r="E27" s="76" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" s="76"/>
+        <v>145</v>
+      </c>
+      <c r="E27" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" s="68"/>
       <c r="G27" t="s">
         <v>27</v>
       </c>
@@ -3769,10 +3960,10 @@
         <v>4</v>
       </c>
       <c r="L27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -3784,26 +3975,26 @@
         <v>308</v>
       </c>
       <c r="Q27" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="44"/>
+      <c r="C28" s="49"/>
       <c r="D28" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="76" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="76"/>
+        <v>146</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="68"/>
       <c r="G28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I28">
         <v>89</v>
@@ -3812,10 +4003,10 @@
         <v>4</v>
       </c>
       <c r="L28" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -3827,21 +4018,21 @@
         <v>308</v>
       </c>
       <c r="Q28" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="44"/>
+      <c r="C29" s="49"/>
       <c r="D29" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="76" t="s">
-        <v>141</v>
-      </c>
-      <c r="F29" s="76"/>
+      <c r="E29" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="68"/>
       <c r="G29" t="s">
         <v>27</v>
       </c>
@@ -3855,10 +4046,10 @@
         <v>4</v>
       </c>
       <c r="L29" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M29" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -3870,21 +4061,56 @@
         <v>308</v>
       </c>
       <c r="Q29" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H32" s="61" t="s">
-        <v>163</v>
-      </c>
-      <c r="I32" s="61"/>
-      <c r="K32" s="62" t="s">
+      <c r="H32" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="I32" s="80"/>
+      <c r="K32" s="81" t="s">
+        <v>161</v>
+      </c>
+      <c r="L32" s="81"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>164</v>
       </c>
-      <c r="L32" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="38">
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B15:R15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="B26:C26"/>
@@ -3893,44 +4119,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="E28:F28"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B15:R15"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="O6:P6"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3941,34 +4129,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E926DD-6A67-4AB9-8E3F-86D623802E50}">
-  <dimension ref="B2:S11"/>
+  <dimension ref="B2:S44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
+      <c r="B2" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -3991,53 +4179,49 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="63">
+      <c r="B4" s="82">
         <v>44627</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="E4" s="63">
+      <c r="C4" s="83"/>
+      <c r="E4" s="82">
         <v>44658</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="H4" s="65" t="s">
+      <c r="F4" s="83"/>
+      <c r="H4" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="K4" s="70" t="s">
+      <c r="I4" s="85"/>
+      <c r="K4" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="71"/>
-      <c r="N4" s="70" t="s">
+      <c r="L4" s="73"/>
+      <c r="N4" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="O4" s="71"/>
-      <c r="Q4" s="70" t="s">
+      <c r="O4" s="73"/>
+      <c r="Q4" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="R4" s="71"/>
+      <c r="R4" s="73"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="M6" s="84" t="s">
+      <c r="N6" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="84"/>
-      <c r="O6" s="83" t="s">
-        <v>135</v>
-      </c>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="R6" s="62"/>
+      <c r="O6" s="90"/>
+      <c r="Q6" s="81" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" s="81"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="74"/>
+      <c r="D8" s="79"/>
       <c r="E8" s="28" t="s">
         <v>114</v>
       </c>
@@ -4056,29 +4240,29 @@
       <c r="K8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="72" t="s">
+      <c r="M8" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72" t="s">
+      <c r="N8" s="88"/>
+      <c r="O8" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72" t="s">
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="R8" s="72"/>
+      <c r="R8" s="88"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="17">
         <v>123456</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -4095,30 +4279,30 @@
       <c r="K9">
         <v>1356</v>
       </c>
-      <c r="M9" s="76" t="s">
+      <c r="M9" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="N9" s="76"/>
-      <c r="O9" s="75">
+      <c r="N9" s="68"/>
+      <c r="O9" s="78">
         <v>44599</v>
       </c>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76" t="s">
-        <v>137</v>
-      </c>
-      <c r="R9" s="76"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="R9" s="68"/>
       <c r="S9" s="22"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="17">
         <v>123456</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="32" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -4135,30 +4319,30 @@
       <c r="K10">
         <v>950</v>
       </c>
-      <c r="M10" s="76" t="s">
+      <c r="M10" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="N10" s="76"/>
-      <c r="O10" s="75">
+      <c r="N10" s="68"/>
+      <c r="O10" s="78">
         <v>44599</v>
       </c>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R10" s="76"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="R10" s="68"/>
       <c r="S10" s="22"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
         <v>123456</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="D11" s="44"/>
+      <c r="C11" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="49"/>
       <c r="E11" s="24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F11">
         <v>15</v>
@@ -4175,22 +4359,755 @@
       <c r="K11">
         <v>3856</v>
       </c>
-      <c r="M11" s="76" t="s">
+      <c r="M11" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="N11" s="76"/>
-      <c r="O11" s="75">
+      <c r="N11" s="68"/>
+      <c r="O11" s="78">
         <v>44599</v>
       </c>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R11" s="76"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="R11" s="68"/>
       <c r="S11" s="22"/>
     </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="36">
+        <v>123457</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="E12" s="96" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12">
+        <v>15</v>
+      </c>
+      <c r="H12" s="21">
+        <v>33026</v>
+      </c>
+      <c r="I12">
+        <v>256</v>
+      </c>
+      <c r="J12">
+        <v>420</v>
+      </c>
+      <c r="K12">
+        <v>3856</v>
+      </c>
+      <c r="M12" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" s="68"/>
+      <c r="O12" s="78">
+        <v>44600</v>
+      </c>
+      <c r="P12" s="68"/>
+      <c r="Q12" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="R12" s="68"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+    </row>
+    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="33"/>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="P17" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q17" s="34"/>
+    </row>
+    <row r="18" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="72"/>
+      <c r="D18" s="73"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
+    </row>
+    <row r="19" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="L19" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="P19" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q19" s="35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="K20" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" t="s">
+        <v>139</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>308</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="I21" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" t="s">
+        <v>151</v>
+      </c>
+      <c r="M21" t="s">
+        <v>139</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>308</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="49"/>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="68"/>
+      <c r="G22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22">
+        <v>308</v>
+      </c>
+      <c r="K22" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>308</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="49"/>
+      <c r="D23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="68"/>
+      <c r="G23" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>459</v>
+      </c>
+      <c r="K23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" t="s">
+        <v>153</v>
+      </c>
+      <c r="M23" t="s">
+        <v>139</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>308</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="49"/>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="68"/>
+      <c r="G24" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>940</v>
+      </c>
+      <c r="K24" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>154</v>
+      </c>
+      <c r="M24" t="s">
+        <v>139</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>308</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="49"/>
+      <c r="D25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="68"/>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25">
+        <v>210</v>
+      </c>
+      <c r="K25" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" t="s">
+        <v>155</v>
+      </c>
+      <c r="M25" t="s">
+        <v>139</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>308</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="68"/>
+      <c r="G26" t="s">
+        <v>147</v>
+      </c>
+      <c r="H26" t="s">
+        <v>148</v>
+      </c>
+      <c r="I26">
+        <v>89</v>
+      </c>
+      <c r="K26" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" t="s">
+        <v>156</v>
+      </c>
+      <c r="M26" t="s">
+        <v>139</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>308</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" s="68"/>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27">
+        <v>18</v>
+      </c>
+      <c r="K27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>157</v>
+      </c>
+      <c r="M27" t="s">
+        <v>139</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>308</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H29" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="I29" s="80"/>
+      <c r="K29" s="81" t="s">
+        <v>161</v>
+      </c>
+      <c r="L29" s="81"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="74"/>
+      <c r="M32" s="74"/>
+      <c r="N32" s="74"/>
+      <c r="O32" s="74"/>
+      <c r="P32" s="74"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="74"/>
+    </row>
+    <row r="33" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" t="s">
+        <v>162</v>
+      </c>
+      <c r="K33" t="s">
+        <v>105</v>
+      </c>
+      <c r="N33" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="69"/>
+      <c r="C34" s="70"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="70"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="70"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="70"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="H36" s="35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>308</v>
+      </c>
+      <c r="H37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>308</v>
+      </c>
+      <c r="H38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>308</v>
+      </c>
+      <c r="H39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>308</v>
+      </c>
+      <c r="H40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>308</v>
+      </c>
+      <c r="H41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>308</v>
+      </c>
+      <c r="H42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C44" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="80"/>
+      <c r="F44" s="81" t="s">
+        <v>161</v>
+      </c>
+      <c r="G44" s="81"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="58">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="B32:R32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B15:R15"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="Q8:R8"/>
     <mergeCell ref="C9:D9"/>
@@ -4202,22 +5119,14 @@
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="M6:N6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="M8:N8"/>
   </mergeCells>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>